<commit_message>
1. Save invoice date 2. Save penalty bookings count
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-CashMain-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-CashMain-v4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>{meta:invoice_type}</t>
   </si>
@@ -150,6 +150,9 @@
   <si>
     <t>Misc 
 Charges</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -490,6 +493,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,6 +511,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,28 +532,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,7 +818,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -843,14 +846,14 @@
     </row>
     <row r="2" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
@@ -974,15 +977,15 @@
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
@@ -1040,13 +1043,15 @@
       <c r="F16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1207,40 +1212,40 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="41"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
       <c r="H30" s="26"/>
       <c r="I30" s="1"/>
     </row>

</xml_diff>

<commit_message>
Bug: Wrong tax rates corrected
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-CashMain-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-CashMain-v4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/templates/anuj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -159,7 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,6 +190,18 @@
       <sz val="18"/>
       <name val="Cambria"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,8 +422,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -539,7 +553,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -818,7 +834,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1130,7 +1146,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="7">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1147,7 +1163,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="7">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1258,5 +1274,6 @@
     <mergeCell ref="D12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>